<commit_message>
defeat, boundaries and flickering implementation
</commit_message>
<xml_diff>
--- a/Features + Mechanics.xlsx
+++ b/Features + Mechanics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ZOO-KEEPER-PICO-8-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFC8B7E-3123-4D33-B783-38760E256D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89E24B2-8196-47BA-93F5-E9EF385502CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27180" yWindow="4170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
recap + small xls addings
</commit_message>
<xml_diff>
--- a/Features + Mechanics.xlsx
+++ b/Features + Mechanics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\ZOO-KEEPER-PICO-8-Game\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ZOO-KEEPER-PICO-8-Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724D4031-19F8-4D23-A581-D5B717F73B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727A1E69-690B-4F75-AC14-57185B22FCC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3612" yWindow="2232" windowWidth="15612" windowHeight="8988" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
   <si>
     <t>Systems</t>
   </si>
@@ -111,18 +111,74 @@
     <t>Player Movement</t>
   </si>
   <si>
-    <t>Live Pickup</t>
-  </si>
-  <si>
     <t>Chase Pickup</t>
+  </si>
+  <si>
+    <t>Life Pickup</t>
+  </si>
+  <si>
+    <t>isChase=true</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Point Pickup</t>
+  </si>
+  <si>
+    <t>Scoring</t>
+  </si>
+  <si>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>State Machine</t>
+  </si>
+  <si>
+    <t>Main Menu state</t>
+  </si>
+  <si>
+    <t>Gameplay state</t>
+  </si>
+  <si>
+    <t>Pause state</t>
+  </si>
+  <si>
+    <t>Defeated state</t>
+  </si>
+  <si>
+    <t>Number of spawns</t>
+  </si>
+  <si>
+    <t>Spawn Rate</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Chaser</t>
+  </si>
+  <si>
+    <t>Spawn Lanes</t>
+  </si>
+  <si>
+    <t>Chasing mode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -150,11 +206,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,39 +492,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -481,7 +538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -492,7 +549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>18</v>
       </c>
@@ -503,23 +560,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -533,16 +596,19 @@
         <v>15</v>
       </c>
       <c r="L7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -550,38 +616,133 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="L12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>3</v>
       </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="L13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" t="s">
-        <v>10</v>
+        <v>32</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>